<commit_message>
Updated Use Case Scenarios
</commit_message>
<xml_diff>
--- a/SystemRequirementsDraft/Rhythmx M.P. Use Case Scenarios.xlsx
+++ b/SystemRequirementsDraft/Rhythmx M.P. Use Case Scenarios.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="psdd7LWUStiUxxfp43oKdKveDUV7kNE1Ubj/S23168E="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="c5RagxpK4k7vbFSw7mMsqdjdRQQ3ffaLfT7DllvHuXA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
   <si>
     <t>Use Case Title</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Precondition:</t>
   </si>
   <si>
-    <t>User must have the app open</t>
+    <t>User must be on a screen that can navigate to the playing screen</t>
   </si>
   <si>
     <t>Postcondition</t>
@@ -56,6 +56,9 @@
     <t>Trigger:</t>
   </si>
   <si>
+    <t>Select a song</t>
+  </si>
+  <si>
     <t>Main Success Scenario:</t>
   </si>
   <si>
@@ -107,7 +110,7 @@
     <t>e. they can enable shuffle play</t>
   </si>
   <si>
-    <t>Open Discover Screen</t>
+    <t>Discover Screen</t>
   </si>
   <si>
     <t>Member must have the app installed</t>
@@ -276,24 +279,57 @@
   </si>
   <si>
     <t>a. they can choose to disable AI features</t>
+  </si>
+  <si>
+    <t>Add friend</t>
+  </si>
+  <si>
+    <t>Other Users</t>
+  </si>
+  <si>
+    <t>User must have the other user's profile displayed</t>
+  </si>
+  <si>
+    <t>The two users are now added as friends</t>
+  </si>
+  <si>
+    <t>Send the other user a friend request</t>
+  </si>
+  <si>
+    <t>User clicks the "add friend" button to send a friend request</t>
+  </si>
+  <si>
+    <t>1.1 System adds a friend request in the other user's inbox</t>
+  </si>
+  <si>
+    <t>1.2 System notifies this other user that they have a friend request</t>
+  </si>
+  <si>
+    <t>Other user accepts the friend request</t>
+  </si>
+  <si>
+    <t>2.1 System makes the two users friends on the app</t>
+  </si>
+  <si>
+    <t>If user accidentally sent a friend request,</t>
+  </si>
+  <si>
+    <t>a. they can click "cancel friend" request</t>
+  </si>
+  <si>
+    <t>b. they can click "remove friend" after the other user has accepted their friend request</t>
+  </si>
+  <si>
+    <t>If other user doesn't want to accept the friend request,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -318,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -326,14 +362,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,7 +599,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -577,7 +607,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -593,7 +623,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -609,7 +639,7 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -617,744 +647,878 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
         <v>1.0</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
-      <c r="C10" s="2" t="s">
-        <v>17</v>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
         <v>2.0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>1.1</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="2" t="s">
-        <v>22</v>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="3" t="s">
-        <v>26</v>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="3" t="s">
-        <v>27</v>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="3" t="s">
-        <v>28</v>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="4"/>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="4"/>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="4"/>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="4"/>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="5">
+      <c r="A32" s="3">
         <v>1.0</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
-        <v>35</v>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="5">
+      <c r="A34" s="3">
         <v>2.0</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="5">
+      <c r="A36" s="3">
         <v>1.1</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="4"/>
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="4"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="4"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="5">
-        <v>1.1</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="4"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="4"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" s="4"/>
+      <c r="B57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="1"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="4"/>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="4"/>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="4"/>
+      <c r="B60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="4"/>
+      <c r="B61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="4"/>
+      <c r="B62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" s="4"/>
+      <c r="B63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="4" t="s">
+      <c r="A64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="B64" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="5">
+      <c r="A65" s="3">
         <v>1.0</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="B65" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C65" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4" t="s">
-        <v>61</v>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4" t="s">
-        <v>62</v>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="5">
+      <c r="A68" s="3">
         <v>2.0</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C68" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="5">
+      <c r="A69" s="3">
         <v>3.0</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C69" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="5">
+      <c r="A71" s="3">
         <v>1.1</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="4"/>
+      <c r="B71" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="4"/>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" s="4"/>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" s="4"/>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="4"/>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="1"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="5">
+      <c r="A76" s="3">
         <v>3.1</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" s="4"/>
+      <c r="B76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C77" s="4"/>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="4"/>
+      <c r="B79" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C80" s="4"/>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C81" s="4"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C82" s="4"/>
+      <c r="B82" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="4"/>
+      <c r="B83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C84" s="4"/>
+      <c r="B84" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C84" s="1"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C85" s="4"/>
+      <c r="B85" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B86" s="4" t="s">
+      <c r="A86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="B86" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C86" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="5">
+      <c r="A87" s="3">
         <v>1.0</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>60</v>
+      <c r="B87" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4" t="s">
-        <v>61</v>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4" t="s">
-        <v>78</v>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="5">
+      <c r="A90" s="3">
         <v>2.0</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C90" s="4" t="s">
+      <c r="B90" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C90" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
+      <c r="A91" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="5">
+      <c r="A92" s="3">
         <v>1.1</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C92" s="4"/>
+      <c r="B92" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C93" s="4"/>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C94" s="4"/>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="5">
+      <c r="A95" s="3">
         <v>1.2</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C95" s="4"/>
+      <c r="B95" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="1"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C96" s="4"/>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" s="1"/>
     </row>
     <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" ht="15.75" customHeight="1">
+      <c r="A99" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" ht="15.75" customHeight="1">
+      <c r="A100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="A101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="A102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" ht="15.75" customHeight="1">
+      <c r="A103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" ht="15.75" customHeight="1">
+      <c r="A104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" ht="15.75" customHeight="1">
+      <c r="A105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="A106" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="107" ht="15.75" customHeight="1">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="A108" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="A109" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="A110" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="A111" s="1"/>
+      <c r="B111" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="A112" s="1"/>
+      <c r="B112" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="A113" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C114" s="1"/>
+    </row>
     <row r="115" ht="15.75" customHeight="1"/>
     <row r="116" ht="15.75" customHeight="1"/>
     <row r="117" ht="15.75" customHeight="1"/>
@@ -2237,7 +2401,6 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>